<commit_message>
ingest: rework jargon, support one-to-many data sources (#1951)
* add string repr for ingest datastore, hybridpathstorage

* move ingest cli out of __init__.py

* add sparse_config to simplify library/datasource/dataset issues

* rename ingest.configure to ingest.plan

* rename templates to definitions

* ingest - one-to-many support and general rework

* cscl gdb ingest definition
</commit_message>
<xml_diff>
--- a/dcpy/test/lifecycle/ingest/resources/test_data/test.xlsx
+++ b/dcpy/test/lifecycle/ingest/resources/test_data/test.xlsx
@@ -489,17 +489,17 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>ZBIhHSAUdsKUqmJewpSS</t>
+          <t>tWlJzrJaXYzgyOCBOLtu</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>-159.331339</t>
+          <t>-179.958101</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>65.482653</t>
+          <t>-2.5592605</t>
         </is>
       </c>
     </row>
@@ -518,17 +518,17 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>EsfswlCbaHEOfMqXFRZU</t>
+          <t>gPcUrDKYsImEbbgIsjvI</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>110.067368</t>
+          <t>106.989965</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>-10.502745</t>
+          <t>64.934071</t>
         </is>
       </c>
     </row>
@@ -555,7 +555,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>QLyTmgxlgZtGHcnjDKSh</t>
+          <t>PoSeWuySWgMXFWTtqxet</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
@@ -580,17 +580,17 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>JexVCnSrRomLXGdQdrZC</t>
+          <t>wKGNGWPcXSdbsqfXZicm</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>102.430992</t>
+          <t>-122.893621</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>-88.0282495</t>
+          <t>1.081778</t>
         </is>
       </c>
     </row>
@@ -613,17 +613,17 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>pIrxJQvpsmnpwXyMirua</t>
+          <t>GpbjzsVxKUVTCvGBLPUF</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>-82.796488</t>
+          <t>-83.086954</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>53.8049295</t>
+          <t>78.3302665</t>
         </is>
       </c>
     </row>

</xml_diff>